<commit_message>
Actualizar atributos de Headers.java
</commit_message>
<xml_diff>
--- a/code/test.xlsx
+++ b/code/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2fee13dea56e37a/Documents/.Workspaces/NAEVYS2 Workspace/NAEVYS/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_8097833108AEAE0E8BD2140C144CB99588D6B5D9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5743B501-6D23-4DA5-9E9B-87064E43E435}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_314AA22E08AEAE0E8BD2140C144CB99558516C36" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{611EE74B-683C-425C-9A2E-EA8C7871FA54}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>This is a string in A1</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
   </si>
 </sst>
 </file>
@@ -56,9 +71,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -74,6 +88,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{225D74EF-B9CF-4688-9BAC-838A54A66791}" name="Table1" displayName="Table1" ref="A1:E2" totalsRowShown="0">
+  <autoFilter ref="A1:E2" xr:uid="{225D74EF-B9CF-4688-9BAC-838A54A66791}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6E3D39AC-2733-4C07-90D4-541601141E14}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{0EF86033-0D37-4A17-9531-10A39A3C6CD9}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{6491A028-E90E-4828-84D6-BEF58C43F0FA}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{2846EE15-F542-445C-B6A7-95B91F350597}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{E1B1E1E1-D957-402F-94F3-B50112FF269C}" name="Column5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,40 +404,58 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>44910.543389351849</v>
-      </c>
-      <c r="C1">
+      <c r="B2">
+        <v>44910.578125254629</v>
+      </c>
+      <c r="C2">
         <v>1234</v>
       </c>
-      <c r="D1">
+      <c r="D2">
         <v>123456</v>
       </c>
-      <c r="E1">
+      <c r="E2">
         <v>1.234</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>